<commit_message>
UI start + random images
</commit_message>
<xml_diff>
--- a/ranges.xlsx
+++ b/ranges.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>eye_aspect_ratio</t>
   </si>
@@ -69,6 +69,51 @@
   </si>
   <si>
     <t>face_aspect_ratio</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>Eye Aspect Ratio</t>
+  </si>
+  <si>
+    <t>Face Aspect Ratio</t>
+  </si>
+  <si>
+    <t>Ear Tip Angle</t>
+  </si>
+  <si>
+    <t>Eye Distance</t>
+  </si>
+  <si>
+    <t>Eye Height</t>
+  </si>
+  <si>
+    <t>Nose Size</t>
+  </si>
+  <si>
+    <t>Whisker Length</t>
+  </si>
+  <si>
+    <t>Ear Angle</t>
+  </si>
+  <si>
+    <t>Ear Point</t>
+  </si>
+  <si>
+    <t>Ear Length</t>
+  </si>
+  <si>
+    <t>Ear Orientation</t>
+  </si>
+  <si>
+    <t>Fur Lightness</t>
+  </si>
+  <si>
+    <t>Fur Saturation</t>
   </si>
 </sst>
 </file>
@@ -412,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,17 +468,24 @@
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,8 +495,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -454,8 +512,14 @@
       <c r="C3">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -465,8 +529,14 @@
       <c r="C4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -477,8 +547,14 @@
         <f>4/3</f>
         <v>1.3333333333333333</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -488,8 +564,14 @@
       <c r="C6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -499,19 +581,31 @@
       <c r="C7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8">
+        <v>-50</v>
+      </c>
+      <c r="C8">
         <v>50</v>
       </c>
-      <c r="C8">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -521,8 +615,14 @@
       <c r="C9">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -532,8 +632,14 @@
       <c r="C10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -543,8 +649,14 @@
       <c r="C11">
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -554,8 +666,14 @@
       <c r="C12">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -565,8 +683,14 @@
       <c r="C13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -575,6 +699,12 @@
       </c>
       <c r="C14">
         <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>